<commit_message>
Update README files with detailed instructions for using the new OKX caching script, including symbol mapping and command execution. Enhance data files for BTC, ETH, and SOL with updated forecasts and predictions. Modify HTML visualizations for improved interactivity and clarity.
</commit_message>
<xml_diff>
--- a/exports/btc-usd_forecast_next7.xlsx
+++ b/exports/btc-usd_forecast_next7.xlsx
@@ -448,71 +448,71 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-11-13</t>
+          <t>2025-11-15</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>101439.65</v>
+        <v>94092.49000000001</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-11-14</t>
+          <t>2025-11-16</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>101466.44</v>
+        <v>94109.49000000001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-11-15</t>
+          <t>2025-11-17</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>101065.6</v>
+        <v>94704.02</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-11-16</t>
+          <t>2025-11-18</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>100996.66</v>
+        <v>94864.87</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-11-17</t>
+          <t>2025-11-19</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>101412.83</v>
+        <v>95273.05</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-11-18</t>
+          <t>2025-11-20</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>101606.51</v>
+        <v>95748.95</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-11-19</t>
+          <t>2025-11-21</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>101549.75</v>
+        <v>95687.57000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>